<commit_message>
index exam formatif S9
</commit_message>
<xml_diff>
--- a/content/projet-final/grille-projet-fil-rouge.xlsx
+++ b/content/projet-final/grille-projet-fil-rouge.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cmontmorency365-my.sharepoint.com/personal/nathalie_desmangles_cmontmorency_qc_ca/Documents/_Automne2024/A24/content/projet-final/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="65" documentId="11_4873821850397D6A206102AB8855B237A12C5B9C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4BB244A8-1256-4215-8A86-001357D2E360}"/>
+  <xr:revisionPtr revIDLastSave="81" documentId="11_4873821850397D6A206102AB8855B237A12C5B9C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9BBB941F-2B2E-4F5E-823A-10EF04ECE6B5}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="0" windowWidth="9780" windowHeight="11370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>Compétence en voie de développement</t>
   </si>
@@ -34,21 +34,6 @@
     <t>Compétence approfondie</t>
   </si>
   <si>
-    <t>Qualité du Code</t>
-  </si>
-  <si>
-    <t>Le code contient de nombreuses erreurs syntaxiques et logiques. Les solutions sont souvent inefficaces.</t>
-  </si>
-  <si>
-    <t>Le code fonctionne mais contient quelques erreurs mineures. Les solutions sont correctes mais peuvent être optimisées.</t>
-  </si>
-  <si>
-    <t>Le code est correct et efficace, avec peu ou pas d’erreurs. Les solutions sont bien pensées.</t>
-  </si>
-  <si>
-    <t>Le code est non seulement correct et efficace, mais aussi élégant et innovant. Les solutions montrent une compréhension approfondie des concepts.</t>
-  </si>
-  <si>
     <t>Les analyses statistiques sont incomplètes ou incorrectes. Les concepts de base ne sont pas bien compris.</t>
   </si>
   <si>
@@ -101,12 +86,6 @@
   </si>
   <si>
     <t>Visualisation des données</t>
-  </si>
-  <si>
-    <t>Documentation et commentaires</t>
-  </si>
-  <si>
-    <t>Utilisation des bibliothèques</t>
   </si>
   <si>
     <t>Niveaux de développement</t>
@@ -132,13 +111,49 @@
   </si>
   <si>
     <t>0 /40</t>
+  </si>
+  <si>
+    <t>Utilisation appropriée des bibliothèques</t>
+  </si>
+  <si>
+    <t>Documentation (commentaires, docstring) judicieuse, claire et précise</t>
+  </si>
+  <si>
+    <t>Respect de la syntaxe et des conventions du langage de programmation</t>
+  </si>
+  <si>
+    <t>Le code contient de nombreuses erreurs syntaxiques et logiques. Les solutions sont souvent inefficaces.
+Les conventions de nomenclature et syntaxiques ne sont pas respectées.</t>
+  </si>
+  <si>
+    <t>Syntaxe correcte et efficace, avec peu ou pas d’erreurs. Les solutions sont bien pensées.
+Respet des conventions nomenclature et de syntaxe dans la grande majorité du temps.</t>
+  </si>
+  <si>
+    <t>Quelques erreurs de syntaxe mineures. Les solutions sont correctes mais peuvent être optimisées.
+Respect partiel des conventions de nomenclature et de syntaxe.</t>
+  </si>
+  <si>
+    <t>Syntaxe impeccable et respect rigoureux des conventions de nomenclature et de syntaxe. Les solutions montrent une compréhension approfondie des concepts.</t>
+  </si>
+  <si>
+    <t>Poids (%)</t>
+  </si>
+  <si>
+    <t>25%</t>
+  </si>
+  <si>
+    <t>Total : 100% (Projet vaut 40% de la note finale)</t>
+  </si>
+  <si>
+    <t>Cette grille permet d’évaluer les projets de manière détaillée et équitable, en tenant compte des différents niveaux de compétence des étudiants. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -161,6 +176,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF111111"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF111111"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -258,7 +286,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -266,37 +294,49 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -638,166 +678,205 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="28.4140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="33.6640625" customWidth="1"/>
     <col min="3" max="3" width="35.33203125" customWidth="1"/>
     <col min="4" max="4" width="33.9140625" customWidth="1"/>
     <col min="5" max="5" width="41.08203125" customWidth="1"/>
+    <col min="6" max="6" width="8.4140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="55.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="55.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+    </row>
+    <row r="2" spans="1:6" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+    </row>
+    <row r="3" spans="1:6" s="1" customFormat="1" ht="48.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="6"/>
+      <c r="B3" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" s="1" customFormat="1" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="6"/>
+      <c r="B4" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" s="1" customFormat="1" ht="94.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" s="1" customFormat="1" ht="94.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="15">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" s="1" customFormat="1" ht="94.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="15">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" s="1" customFormat="1" ht="94.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-    </row>
-    <row r="2" spans="1:5" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A2" s="4" t="s">
+      <c r="B8" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="15">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" s="1" customFormat="1" ht="94.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-    </row>
-    <row r="3" spans="1:5" s="1" customFormat="1" ht="48.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="8"/>
-      <c r="B3" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" s="1" customFormat="1" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="8"/>
-      <c r="B4" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" s="1" customFormat="1" ht="94.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" s="1" customFormat="1" ht="94.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" s="1" customFormat="1" ht="94.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" s="7" t="s">
+      <c r="B9" s="11" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" s="1" customFormat="1" ht="94.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="B8" s="13" t="s">
+      <c r="C9" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="D9" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="E9" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" s="1" customFormat="1" ht="94.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B9" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>24</v>
-      </c>
+      <c r="F9" s="15">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="23" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" s="16"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+    </row>
+    <row r="12" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" s="17"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B1:E1"/>
+    <mergeCell ref="A11:E11"/>
+    <mergeCell ref="A12:E12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A5:E5 B9:E9 B6:E6 B7:E7 B8:E8 B3:E3" numberStoredAsText="1"/>
+    <ignoredError sqref="B9:E9 B6:E6 B7:E7 B8:E8 F5" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>